<commit_message>
changed color of instructions
</commit_message>
<xml_diff>
--- a/TrackMeNow.xlsx
+++ b/TrackMeNow.xlsx
@@ -376,9 +376,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -397,6 +394,9 @@
     <xf numFmtId="20" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="220">
@@ -1013,7 +1013,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="17" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="2" customWidth="1"/>
     <col min="5" max="5" width="12" style="6" bestFit="1" customWidth="1"/>
@@ -1022,12 +1022,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1">
-      <c r="A1" s="17" t="str">
+      <c r="A1" s="22" t="str">
         <f>IF(ISBLANK(B2),"(Type how long you'd like to work today, ex: 7:00) ⇘",IF(ISBLANK(B3),"(Type how long you plan to be on break, ex: 2:00) ⇘","(Use Ctrl+Shift+, to add the current time) ⇘"))</f>
         <v>(Type how long you'd like to work today, ex: 7:00) ⇘</v>
       </c>
       <c r="C1" s="8"/>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22"/>
+      <c r="B2" s="21"/>
       <c r="D2" s="4" t="str">
         <f>IF(NOT(ISBLANK(B2)),"which means I will be done at","")</f>
         <v/>
@@ -1054,7 +1054,7 @@
         <f>IF(NOT(ISBLANK(B2)),"and take several breaks totaling","")</f>
         <v/>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="20"/>
       <c r="D3" s="3" t="str">
         <f>IF(NOT(ISBLANK(B5)),"So far, I have spent","")</f>
         <v/>
@@ -1092,7 +1092,7 @@
         <f>IF(NOT(ISBLANK(B4)),"and took a break at","")</f>
         <v/>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B5)),NOT(ISBLANK(B4))),B5-B4,"")</f>
         <v/>
@@ -1114,7 +1114,7 @@
         <f>IF(NOT(ISBLANK(B6)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B7)),NOT(ISBLANK(B6))),B7-B6,"")</f>
         <v/>
@@ -1136,7 +1136,7 @@
         <f t="shared" ref="A9:A21" si="1">IF(NOT(ISBLANK(B8)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B9)),NOT(ISBLANK(B8))),B9-B8,"")</f>
         <v/>
@@ -1158,7 +1158,7 @@
         <f t="shared" ref="A11:A21" si="3">IF(NOT(ISBLANK(B10)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B11)),NOT(ISBLANK(B10))),B11-B10,"")</f>
         <v/>
@@ -1180,7 +1180,7 @@
         <f t="shared" ref="A13:A21" si="5">IF(NOT(ISBLANK(B12)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B13)),NOT(ISBLANK(B12))),B13-B12,"")</f>
         <v/>
@@ -1202,7 +1202,7 @@
         <f t="shared" ref="A15:A21" si="7">IF(NOT(ISBLANK(B14)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B15)),NOT(ISBLANK(B14))),B15-B14,"")</f>
         <v/>
@@ -1226,7 +1226,7 @@
         <f t="shared" ref="A17:A21" si="9">IF(NOT(ISBLANK(B16)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B17)),NOT(ISBLANK(B16))),B17-B16,"")</f>
         <v/>
@@ -1250,7 +1250,7 @@
         <f t="shared" ref="A19:A21" si="11">IF(NOT(ISBLANK(B18)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B19)),NOT(ISBLANK(B18))),B19-B18,"")</f>
         <v/>
@@ -1274,7 +1274,7 @@
         <f t="shared" ref="A21" si="13">IF(NOT(ISBLANK(B20)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B21" s="21"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="12" t="str">
         <f>IF(AND(NOT(ISBLANK(B21)),NOT(ISBLANK(B20))),B21-B20,"")</f>
         <v/>
@@ -1297,7 +1297,7 @@
       <c r="D23" s="1"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" s="19"/>
+      <c r="B32" s="18"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
unlocked most cells, changed Done message
</commit_message>
<xml_diff>
--- a/TrackMeNow.xlsx
+++ b/TrackMeNow.xlsx
@@ -33,12 +33,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="165" formatCode="[&lt;11]&quot;Low&quot;* 0;[&gt;20]&quot;High&quot;* 0;&quot;Average&quot;* 0"/>
-    <numFmt numFmtId="167" formatCode="&quot;which means I will be done by&quot;\ h:mm"/>
-    <numFmt numFmtId="169" formatCode="[&lt;0.0416]\([m]\ &quot;min working)&quot;;&quot;(&quot;[h]\:mm\ &quot;hours working)&quot;"/>
-    <numFmt numFmtId="170" formatCode="[&lt;0.0416][m]\ &quot;min&quot;;[h]:mm\ &quot;hours&quot;"/>
-    <numFmt numFmtId="172" formatCode="[&lt;0.0416]&quot;(&quot;[m]\ &quot;min later)&quot;;&quot;(&quot;[h]\:mm\ &quot;hours later)&quot;"/>
-    <numFmt numFmtId="173" formatCode="[&lt;0.0416]\([m]\ &quot;min left)&quot;;\([h]:mm\ &quot;hours left&quot;\)"/>
+    <numFmt numFmtId="164" formatCode="[&lt;11]&quot;Low&quot;* 0;[&gt;20]&quot;High&quot;* 0;&quot;Average&quot;* 0"/>
+    <numFmt numFmtId="165" formatCode="&quot;which means I will be done by&quot;\ h:mm"/>
+    <numFmt numFmtId="166" formatCode="[&lt;0.0416]\([m]\ &quot;min working)&quot;;&quot;(&quot;[h]\:mm\ &quot;hours working)&quot;"/>
+    <numFmt numFmtId="167" formatCode="[&lt;0.0416][m]\ &quot;min&quot;;[h]:mm\ &quot;hours&quot;"/>
+    <numFmt numFmtId="168" formatCode="[&lt;0.0416]&quot;(&quot;[m]\ &quot;min later)&quot;;&quot;(&quot;[h]\:mm\ &quot;hours later)&quot;"/>
+    <numFmt numFmtId="169" formatCode="[&lt;0.0416]\([m]\ &quot;min left)&quot;;\([h]:mm\ &quot;hours left&quot;\)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -329,49 +329,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="173" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -380,12 +339,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="219" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,8 +351,65 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="219" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="220">
@@ -1012,292 +1025,295 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="29.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1">
-      <c r="A1" s="22" t="str">
+      <c r="A1" s="11" t="str">
         <f>IF(ISBLANK(B2),"(Type how long you'd like to work today, ex: 7:00) ⇘",IF(ISBLANK(B3),"(Type how long you plan to be on break, ex: 2:00) ⇘","(Use Ctrl+Shift+, to add the current time) ⇘"))</f>
         <v>(Type how long you'd like to work today, ex: 7:00) ⇘</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="6"/>
+      <c r="F1" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="D2" s="4" t="str">
+      <c r="B2" s="5"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16" t="str">
         <f>IF(NOT(ISBLANK(B2)),"which means I will be done at","")</f>
         <v/>
       </c>
-      <c r="E2" s="14" t="str">
+      <c r="E2" s="17" t="str">
         <f ca="1">IF(NOT(ISBLANK(B2)),NOW()+B2+B3,"")</f>
         <v/>
       </c>
-      <c r="F2" s="13" t="str">
-        <f>IF(NOT(ISBLANK(B2)),IF(NOT(E3=""),IF(B2-E3&gt;0,B2-E3,"(Done, go have fun!)"),B2),"")</f>
+      <c r="F2" s="18" t="str">
+        <f>IF(NOT(ISBLANK(B2)),IF(NOT(E3=""),IF(B2-E3&gt;0,B2-E3,"(Done!)"),B2),"")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="12" t="str">
         <f>IF(NOT(ISBLANK(B2)),"and take several breaks totaling","")</f>
         <v/>
       </c>
-      <c r="B3" s="20"/>
-      <c r="D3" s="3" t="str">
+      <c r="B3" s="4"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="19" t="str">
         <f>IF(NOT(ISBLANK(B5)),"So far, I have spent","")</f>
         <v/>
       </c>
-      <c r="E3" s="15" t="str">
+      <c r="E3" s="20" t="str">
         <f>IF(NOT(ISBLANK(B5)),SUM(C5,C7,C9,C11,C13,C15,C17,C19,C21),"")</f>
         <v/>
       </c>
-      <c r="F3" s="8" t="str">
+      <c r="F3" s="21" t="str">
         <f>IF(NOT(ISBLANK(B5)),"working","")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="10" t="str">
+      <c r="A4" s="13" t="str">
         <f>IF(NOT(ISBLANK(B3)),"I started working at","")</f>
         <v/>
       </c>
-      <c r="B4" s="16"/>
-      <c r="D4" s="3" t="str">
+      <c r="B4" s="1"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="19" t="str">
         <f>IF(NOT(ISBLANK(B6)),"and","")</f>
         <v/>
       </c>
-      <c r="E4" s="15" t="str">
+      <c r="E4" s="20" t="str">
         <f>IF(NOT(ISBLANK(B6)),SUM(C6,C8,C10,C12,C14,C16,C18,C20,C22),"")</f>
         <v/>
       </c>
-      <c r="F4" s="8" t="str">
+      <c r="F4" s="21" t="str">
         <f>IF(NOT(ISBLANK(B6)),"resting","")</f>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="12" t="str">
         <f>IF(NOT(ISBLANK(B4)),"and took a break at","")</f>
         <v/>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="12" t="str">
+      <c r="B5" s="4"/>
+      <c r="C5" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B5)),NOT(ISBLANK(B4))),B5-B4,"")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="11" t="str">
+      <c r="A6" s="14" t="str">
         <f>IF(NOT(ISBLANK(B5)),"Then I went back to work at","")</f>
         <v/>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="9" t="str">
+      <c r="B6" s="1"/>
+      <c r="C6" s="23" t="str">
         <f>IF(NOT(ISBLANK(B6)),B6-B5,"")</f>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="12" t="str">
         <f>IF(NOT(ISBLANK(B6)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="12" t="str">
+      <c r="B7" s="4"/>
+      <c r="C7" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B7)),NOT(ISBLANK(B6))),B7-B6,"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="11" t="str">
-        <f t="shared" ref="A8:A21" si="0">IF(NOT(ISBLANK(B7)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="9" t="str">
+      <c r="A8" s="14" t="str">
+        <f t="shared" ref="A8" si="0">IF(NOT(ISBLANK(B7)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="23" t="str">
         <f>IF(NOT(ISBLANK(B8)),B8-B7,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="5" t="str">
-        <f t="shared" ref="A9:A21" si="1">IF(NOT(ISBLANK(B8)),"and took the next break at","")</f>
-        <v/>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="12" t="str">
+      <c r="A9" s="12" t="str">
+        <f t="shared" ref="A9" si="1">IF(NOT(ISBLANK(B8)),"and took the next break at","")</f>
+        <v/>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B9)),NOT(ISBLANK(B8))),B9-B8,"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="11" t="str">
-        <f t="shared" ref="A10:A21" si="2">IF(NOT(ISBLANK(B9)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="9" t="str">
+      <c r="A10" s="14" t="str">
+        <f t="shared" ref="A10" si="2">IF(NOT(ISBLANK(B9)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="23" t="str">
         <f>IF(NOT(ISBLANK(B10)),B10-B9,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="5" t="str">
-        <f t="shared" ref="A11:A21" si="3">IF(NOT(ISBLANK(B10)),"and took the next break at","")</f>
-        <v/>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="12" t="str">
+      <c r="A11" s="12" t="str">
+        <f t="shared" ref="A11" si="3">IF(NOT(ISBLANK(B10)),"and took the next break at","")</f>
+        <v/>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B11)),NOT(ISBLANK(B10))),B11-B10,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="11" t="str">
-        <f t="shared" ref="A12:A21" si="4">IF(NOT(ISBLANK(B11)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="9" t="str">
+      <c r="A12" s="14" t="str">
+        <f t="shared" ref="A12" si="4">IF(NOT(ISBLANK(B11)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="23" t="str">
         <f>IF(NOT(ISBLANK(B12)),B12-B11,"")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5" t="str">
-        <f t="shared" ref="A13:A21" si="5">IF(NOT(ISBLANK(B12)),"and took the next break at","")</f>
-        <v/>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="12" t="str">
+      <c r="A13" s="12" t="str">
+        <f t="shared" ref="A13" si="5">IF(NOT(ISBLANK(B12)),"and took the next break at","")</f>
+        <v/>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B13)),NOT(ISBLANK(B12))),B13-B12,"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="11" t="str">
-        <f t="shared" ref="A14:A21" si="6">IF(NOT(ISBLANK(B13)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="9" t="str">
+      <c r="A14" s="14" t="str">
+        <f t="shared" ref="A14" si="6">IF(NOT(ISBLANK(B13)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="23" t="str">
         <f>IF(NOT(ISBLANK(B14)),B14-B13,"")</f>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="5" t="str">
-        <f t="shared" ref="A15:A21" si="7">IF(NOT(ISBLANK(B14)),"and took the next break at","")</f>
-        <v/>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="12" t="str">
+      <c r="A15" s="12" t="str">
+        <f t="shared" ref="A15" si="7">IF(NOT(ISBLANK(B14)),"and took the next break at","")</f>
+        <v/>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B15)),NOT(ISBLANK(B14))),B15-B14,"")</f>
         <v/>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="11" t="str">
-        <f t="shared" ref="A16:A21" si="8">IF(NOT(ISBLANK(B15)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="9" t="str">
+      <c r="A16" s="14" t="str">
+        <f t="shared" ref="A16" si="8">IF(NOT(ISBLANK(B15)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="23" t="str">
         <f>IF(NOT(ISBLANK(B16)),B16-B15,"")</f>
         <v/>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="5" t="str">
-        <f t="shared" ref="A17:A21" si="9">IF(NOT(ISBLANK(B16)),"and took the next break at","")</f>
-        <v/>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="12" t="str">
+      <c r="A17" s="12" t="str">
+        <f t="shared" ref="A17" si="9">IF(NOT(ISBLANK(B16)),"and took the next break at","")</f>
+        <v/>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B17)),NOT(ISBLANK(B16))),B17-B16,"")</f>
         <v/>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="11" t="str">
-        <f t="shared" ref="A18:A21" si="10">IF(NOT(ISBLANK(B17)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="9" t="str">
+      <c r="A18" s="14" t="str">
+        <f t="shared" ref="A18" si="10">IF(NOT(ISBLANK(B17)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="23" t="str">
         <f>IF(NOT(ISBLANK(B18)),B18-B17,"")</f>
         <v/>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="5" t="str">
-        <f t="shared" ref="A19:A21" si="11">IF(NOT(ISBLANK(B18)),"and took the next break at","")</f>
-        <v/>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="12" t="str">
+      <c r="A19" s="12" t="str">
+        <f t="shared" ref="A19" si="11">IF(NOT(ISBLANK(B18)),"and took the next break at","")</f>
+        <v/>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B19)),NOT(ISBLANK(B18))),B19-B18,"")</f>
         <v/>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="11" t="str">
-        <f t="shared" ref="A20:A21" si="12">IF(NOT(ISBLANK(B19)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="9" t="str">
+      <c r="A20" s="14" t="str">
+        <f t="shared" ref="A20" si="12">IF(NOT(ISBLANK(B19)),"Then I went back to work at","")</f>
+        <v/>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="23" t="str">
         <f>IF(NOT(ISBLANK(B20)),B20-B19,"")</f>
         <v/>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="5" t="str">
+      <c r="A21" s="12" t="str">
         <f t="shared" ref="A21" si="13">IF(NOT(ISBLANK(B20)),"and took the next break at","")</f>
         <v/>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="12" t="str">
+      <c r="B21" s="4"/>
+      <c r="C21" s="22" t="str">
         <f>IF(AND(NOT(ISBLANK(B21)),NOT(ISBLANK(B20))),B21-B20,"")</f>
         <v/>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="11" t="str">
+      <c r="A22" s="14" t="str">
         <f>IF(NOT(ISBLANK(B21)),"Then I went back to work at","")</f>
         <v/>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="9" t="str">
+      <c r="B22" s="1"/>
+      <c r="C22" s="23" t="str">
         <f>IF(NOT(ISBLANK(B22)),B22-B21,"")</f>
         <v/>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="D23" s="1"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="B32" s="18"/>
+      <c r="B32" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
changed readme, fixed bugs
</commit_message>
<xml_diff>
--- a/TrackMeNow.xlsx
+++ b/TrackMeNow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="10540" windowWidth="38400" windowHeight="10540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TrackMeNow" sheetId="1" r:id="rId1"/>
@@ -32,13 +32,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[&lt;11]&quot;Low&quot;* 0;[&gt;20]&quot;High&quot;* 0;&quot;Average&quot;* 0"/>
     <numFmt numFmtId="165" formatCode="&quot;which means I will be done by&quot;\ h:mm"/>
     <numFmt numFmtId="166" formatCode="[&lt;0.0416]\([m]\ &quot;min working)&quot;;&quot;(&quot;[h]\:mm\ &quot;hours working)&quot;"/>
     <numFmt numFmtId="167" formatCode="[&lt;0.0416][m]\ &quot;min&quot;;[h]:mm\ &quot;hours&quot;"/>
     <numFmt numFmtId="168" formatCode="[&lt;0.0416]&quot;(&quot;[m]\ &quot;min later)&quot;;&quot;(&quot;[h]\:mm\ &quot;hours later)&quot;"/>
-    <numFmt numFmtId="169" formatCode="[&lt;0.0416]\([m]\ &quot;min left)&quot;;\([h]:mm\ &quot;hours left&quot;\)"/>
+    <numFmt numFmtId="169" formatCode="[&lt;0.0416]&quot;(&quot;[m]\ &quot;min left),&quot;;&quot;(&quot;[h]:mm\ &quot;hours left),&quot;"/>
+    <numFmt numFmtId="170" formatCode="[&lt;0.0416]&quot;(&quot;[m]\ &quot;min still available).&quot;;&quot;(&quot;[h]:mm\ &quot;hours still available).&quot;"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -107,7 +108,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="220">
+  <cellStyleXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -328,6 +329,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -351,68 +354,61 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="219" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="220">
+  <cellStyles count="222">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -522,6 +518,8 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1025,22 +1023,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="29.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="33" customHeight="1">
-      <c r="A1" s="11" t="str">
-        <f>IF(ISBLANK(B2),"(Type how long you'd like to work today, ex: 7:00) ⇘",IF(ISBLANK(B3),"(Type how long you plan to be on break, ex: 2:00) ⇘","(Use Ctrl+Shift+, to add the current time) ⇘"))</f>
-        <v>(Type how long you'd like to work today, ex: 7:00) ⇘</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="F1" s="24" t="s">
+      <c r="A1" s="8" t="str">
+        <f>IF(ISBLANK(B2),"(Type how long you would like to work today, ex: 7:00) ⇘",IF(ISBLANK(B3),"(Type how long you plan to be on break, ex: 2:00) ⇘","(Use “Ctrl Shift ,” to add the current time) ⇘"))</f>
+        <v>(Type how long you would like to work today, ex: 7:00) ⇘</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="F1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1049,17 +1047,12 @@
         <v>0</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="str">
-        <f>IF(NOT(ISBLANK(B2)),"which means I will be done at","")</f>
-        <v/>
-      </c>
-      <c r="E2" s="17" t="str">
-        <f ca="1">IF(NOT(ISBLANK(B2)),NOW()+B2+B3,"")</f>
-        <v/>
-      </c>
-      <c r="F2" s="18" t="str">
-        <f>IF(NOT(ISBLANK(B2)),IF(NOT(E3=""),IF(B2-E3&gt;0,B2-E3,"(Done!)"),B2),"")</f>
+      <c r="D2" s="14" t="str">
+        <f>IF(NOT(ISBLANK(B2)),IF(E2="","","which means I will be done by"),"")</f>
+        <v/>
+      </c>
+      <c r="E2" s="15" t="str">
+        <f ca="1">IF(NOT(ISBLANK(B2)),IF(F3="",NOW()+B2+B3,IF(F4="",NOW()+F3+B3,IF(B3-E4&gt;0,IF(ISNUMBER(F3),NOW()+F3+F4,""),IF(ISNUMBER(F3),NOW()+F3,"")))),"")</f>
         <v/>
       </c>
     </row>
@@ -1069,37 +1062,35 @@
         <v/>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="19" t="str">
-        <f>IF(NOT(ISBLANK(B5)),"So far, I have spent","")</f>
-        <v/>
-      </c>
-      <c r="E3" s="20" t="str">
+      <c r="D3" s="17" t="str">
+        <f>IF(NOT(ISBLANK(B5)),"So far, I have been working for","")</f>
+        <v/>
+      </c>
+      <c r="E3" s="18" t="str">
         <f>IF(NOT(ISBLANK(B5)),SUM(C5,C7,C9,C11,C13,C15,C17,C19,C21),"")</f>
         <v/>
       </c>
-      <c r="F3" s="21" t="str">
-        <f>IF(NOT(ISBLANK(B5)),"working","")</f>
+      <c r="F3" s="19" t="str">
+        <f>IF(NOT(ISBLANK(B2)),IF(NOT(E3=""),IF(B2-E3&gt;0,B2-E3,"(done for the day),"),""),"")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13" t="str">
+      <c r="A4" s="20" t="str">
         <f>IF(NOT(ISBLANK(B3)),"I started working at","")</f>
         <v/>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="19" t="str">
-        <f>IF(NOT(ISBLANK(B6)),"and","")</f>
-        <v/>
-      </c>
-      <c r="E4" s="20" t="str">
-        <f>IF(NOT(ISBLANK(B6)),SUM(C6,C8,C10,C12,C14,C16,C18,C20,C22),"")</f>
+      <c r="D4" s="17" t="str">
+        <f>IF(NOT(ISBLANK(B5)),"and been on a break for","")</f>
+        <v/>
+      </c>
+      <c r="E4" s="18" t="str">
+        <f>IF(NOT(ISBLANK(B5)),SUM(C6,C8,C10,C12,C14,C16,C18,C20),"")</f>
         <v/>
       </c>
       <c r="F4" s="21" t="str">
-        <f>IF(NOT(ISBLANK(B6)),"resting","")</f>
+        <f>IF(NOT(ISBLANK(B3)),IF(NOT(E4=""),IF(B3-E4&gt;0,B3-E4,"(no more breaks)."),""),"")</f>
         <v/>
       </c>
     </row>
@@ -1110,18 +1101,18 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B5)),NOT(ISBLANK(B4))),B5-B4,"")</f>
+        <f>IF(AND(NOT(ISBLANK(B5)),NOT(ISBLANK(B4))),IF(B5&gt;=B4,B5-B4,B5+1-B4),"")</f>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="14" t="str">
+      <c r="A6" s="23" t="str">
         <f>IF(NOT(ISBLANK(B5)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B6)),B6-B5,"")</f>
+      <c r="C6" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B6)),IF(B6&gt;=B5,B6-B5,B6+1-B5),"")</f>
         <v/>
       </c>
     </row>
@@ -1132,18 +1123,18 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B7)),NOT(ISBLANK(B6))),B7-B6,"")</f>
+        <f>IF(AND(NOT(ISBLANK(B7)),NOT(ISBLANK(B6))),IF(B7&gt;=B6,B7-B6,B7+1-B6),"")</f>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="14" t="str">
+      <c r="A8" s="23" t="str">
         <f t="shared" ref="A8" si="0">IF(NOT(ISBLANK(B7)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B8)),B8-B7,"")</f>
+      <c r="C8" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B8)),IF(B8&gt;=B7,B8-B7,B8+1-B7),"")</f>
         <v/>
       </c>
     </row>
@@ -1154,18 +1145,18 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B9)),NOT(ISBLANK(B8))),B9-B8,"")</f>
+        <f>IF(AND(NOT(ISBLANK(B9)),NOT(ISBLANK(B8))),IF(B9&gt;=B8,B9-B8,B9+1-B8),"")</f>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="14" t="str">
+      <c r="A10" s="23" t="str">
         <f t="shared" ref="A10" si="2">IF(NOT(ISBLANK(B9)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B10)),B10-B9,"")</f>
+      <c r="C10" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B10)),IF(B10&gt;=B9,B10-B9,B10+1-B9),"")</f>
         <v/>
       </c>
     </row>
@@ -1176,18 +1167,18 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B11)),NOT(ISBLANK(B10))),B11-B10,"")</f>
+        <f>IF(AND(NOT(ISBLANK(B11)),NOT(ISBLANK(B10))),IF(B11&gt;=B10,B11-B10,B11+1-B10),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="14" t="str">
+      <c r="A12" s="23" t="str">
         <f t="shared" ref="A12" si="4">IF(NOT(ISBLANK(B11)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B12)),B12-B11,"")</f>
+      <c r="C12" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B12)),IF(B12&gt;=B11,B12-B11,B12+1-B11),"")</f>
         <v/>
       </c>
     </row>
@@ -1198,18 +1189,18 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B13)),NOT(ISBLANK(B12))),B13-B12,"")</f>
+        <f>IF(AND(NOT(ISBLANK(B13)),NOT(ISBLANK(B12))),IF(B13&gt;=B12,B13-B12,B13+1-B12),"")</f>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="14" t="str">
+      <c r="A14" s="23" t="str">
         <f t="shared" ref="A14" si="6">IF(NOT(ISBLANK(B13)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B14)),B14-B13,"")</f>
+      <c r="C14" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B14)),IF(B14&gt;=B13,B14-B13,B14+1-B13),"")</f>
         <v/>
       </c>
     </row>
@@ -1220,22 +1211,22 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B15)),NOT(ISBLANK(B14))),B15-B14,"")</f>
-        <v/>
-      </c>
-      <c r="D15" s="9"/>
+        <f>IF(AND(NOT(ISBLANK(B15)),NOT(ISBLANK(B14))),IF(B15&gt;=B14,B15-B14,B15+1-B14),"")</f>
+        <v/>
+      </c>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="14" t="str">
+      <c r="A16" s="23" t="str">
         <f t="shared" ref="A16" si="8">IF(NOT(ISBLANK(B15)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B16)),B16-B15,"")</f>
-        <v/>
-      </c>
-      <c r="D16" s="9"/>
+      <c r="C16" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B16)),IF(B16&gt;=B15,B16-B15,B16+1-B15),"")</f>
+        <v/>
+      </c>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="12" t="str">
@@ -1244,22 +1235,22 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B17)),NOT(ISBLANK(B16))),B17-B16,"")</f>
-        <v/>
-      </c>
-      <c r="D17" s="9"/>
+        <f>IF(AND(NOT(ISBLANK(B17)),NOT(ISBLANK(B16))),IF(B17&gt;=B16,B17-B16,B17+1-B16),"")</f>
+        <v/>
+      </c>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="14" t="str">
+      <c r="A18" s="23" t="str">
         <f t="shared" ref="A18" si="10">IF(NOT(ISBLANK(B17)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B18)),B18-B17,"")</f>
-        <v/>
-      </c>
-      <c r="D18" s="9"/>
+      <c r="C18" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B18)),IF(B18&gt;=B17,B18-B17,B18+1-B17),"")</f>
+        <v/>
+      </c>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="str">
@@ -1268,22 +1259,22 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B19)),NOT(ISBLANK(B18))),B19-B18,"")</f>
-        <v/>
-      </c>
-      <c r="D19" s="9"/>
+        <f>IF(AND(NOT(ISBLANK(B19)),NOT(ISBLANK(B18))),IF(B19&gt;=B18,B19-B18,B19+1-B18),"")</f>
+        <v/>
+      </c>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="14" t="str">
+      <c r="A20" s="23" t="str">
         <f t="shared" ref="A20" si="12">IF(NOT(ISBLANK(B19)),"Then I went back to work at","")</f>
         <v/>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B20)),B20-B19,"")</f>
-        <v/>
-      </c>
-      <c r="D20" s="9"/>
+      <c r="C20" s="24" t="str">
+        <f>IF(NOT(ISBLANK(B20)),IF(B20&gt;=B19,B20-B19,B20+1-B19),"")</f>
+        <v/>
+      </c>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="12" t="str">
@@ -1292,54 +1283,47 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="22" t="str">
-        <f>IF(AND(NOT(ISBLANK(B21)),NOT(ISBLANK(B20))),B21-B20,"")</f>
-        <v/>
-      </c>
-      <c r="D21" s="9"/>
+        <f>IF(AND(NOT(ISBLANK(B21)),NOT(ISBLANK(B20))),IF(B21&gt;=B20,B21-B20,B21+1-B20),"")</f>
+        <v/>
+      </c>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="14" t="str">
-        <f>IF(NOT(ISBLANK(B21)),"Then I went back to work at","")</f>
-        <v/>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="23" t="str">
-        <f>IF(NOT(ISBLANK(B22)),B22-B21,"")</f>
-        <v/>
-      </c>
-      <c r="D22" s="9"/>
+      <c r="A22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="16"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="D23" s="9"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="32" spans="1:4">
       <c r="B32" s="3"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
-      <formula>AND(B4&lt;&gt;"",B5="")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="B6 B8 B10 B12 B14 B16 B18 B20">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AND(B5&lt;&gt;"",B6="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B22">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="B7 B9 B11 B13 B15 B17 B19 B21">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>AND(B6&lt;&gt;"",B7="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>AND(B2&lt;&gt;"",B3="")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>AND(B2="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+      <formula>AND(B4&lt;&gt;"",B5="")</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>